<commit_message>
ASPE 2024 Annual Conference Release
ASPE 2024 Annual Conference Release:
1. Simplified functions to solve KC system to take KC object. One function fetches config file and creates KC object and the other solves the KC system.
2. Fixed bug where for nonsymmetric KC's, the vee positions were shifted from the ball positions. Issue related to transforming the KC object, vee transforms were previously only rotated instead of by position and rotation.
3. Verified force balance equations are correct. Force balance equations from Precision Machine Design (Slocum, 1992) included a typo discovered by both Seawright and Rojas independently.
4. Removed junk files from directory. Added tutorial script. Added generic 2D and 3D coupling configurations. Added fused silica material.
5. Started adding friction and repeatability to model. Currently WIP and not accessible.
</commit_message>
<xml_diff>
--- a/Material_Lib.xlsx
+++ b/Material_Lib.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kla-my.sharepoint.com/personal/tyler_seawright_kla-tencor_com/Documents/Documents/KC_SOLVER/KC_SOLVER_MATLAB, 7-1-24/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kla-my.sharepoint.com/personal/tyler_seawright_kla-tencor_com/Documents/Documents/KC_SOLVER/KC_SOLVER_MATLAB, DEV, 10-07-24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{D084C576-A0B3-4C70-95A2-870EE24B3C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A70D1904-9BD1-47FD-A2F2-B83145C027D3}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{D084C576-A0B3-4C70-95A2-870EE24B3C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26AD9829-AA67-4E79-A25D-ECA6B0DBB3F9}"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="4275" windowWidth="21600" windowHeight="11385" xr2:uid="{AB6D655C-35F1-4EA9-9A07-18AB4D133046}"/>
+    <workbookView xWindow="5355" yWindow="2955" windowWidth="21600" windowHeight="12735" xr2:uid="{AB6D655C-35F1-4EA9-9A07-18AB4D133046}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Material</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Fused Silica</t>
+  </si>
+  <si>
+    <t>Delrin</t>
+  </si>
+  <si>
+    <t>NBK7</t>
   </si>
 </sst>
 </file>
@@ -130,7 +136,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC92BDF-74A4-43A5-8500-0D719523E848}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +464,7 @@
     <col min="3" max="3" width="25.28515625" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
     <col min="5" max="5" width="25.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -477,7 +483,7 @@
       <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -492,13 +498,13 @@
         <v>276000000</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D9" si="0">B2/(2*(1+F2))</f>
+        <f t="shared" ref="D2:D13" si="0">B2/(2*(1+F2))</f>
         <v>25902255639.097744</v>
       </c>
       <c r="E2" s="1">
         <v>207000000</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>0.33</v>
       </c>
     </row>
@@ -540,7 +546,7 @@
       <c r="E4" s="1">
         <v>280000000</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>0.28999999999999998</v>
       </c>
     </row>
@@ -562,7 +568,7 @@
         <f>0.75*C5</f>
         <v>352500000</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>0.28999999999999998</v>
       </c>
     </row>
@@ -577,12 +583,13 @@
         <v>276000000</v>
       </c>
       <c r="D6" s="1">
-        <v>25900000000</v>
+        <f t="shared" si="0"/>
+        <v>79069767441.860458</v>
       </c>
       <c r="E6" s="1">
         <v>207000000</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="2">
         <v>0.28999999999999998</v>
       </c>
     </row>
@@ -601,10 +608,10 @@
         <v>25930232558.139534</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" ref="E7:E11" si="1">0.75*C7</f>
+        <f t="shared" ref="E7:E13" si="1">0.75*C7</f>
         <v>258750000</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>0.28999999999999998</v>
       </c>
     </row>
@@ -648,7 +655,7 @@
         <f t="shared" si="1"/>
         <v>3450</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>0.14000000000000001</v>
       </c>
     </row>
@@ -663,14 +670,14 @@
         <v>1404000000</v>
       </c>
       <c r="D10" s="1">
-        <f>B10/(2*(1+F10))</f>
+        <f t="shared" si="0"/>
         <v>276446280991.73553</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="1"/>
+        <f>0.75*C10</f>
         <v>1053000000</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>0.21</v>
       </c>
     </row>
@@ -685,24 +692,63 @@
         <v>152200000</v>
       </c>
       <c r="D11" s="1">
-        <v>30800000000</v>
+        <f t="shared" si="0"/>
+        <v>30956521739.130436</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="1"/>
         <v>114150000</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="2">
         <v>0.15</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="1"/>
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1">
+        <v>72000000000</v>
+      </c>
+      <c r="C12" s="1">
+        <v>48000000</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>30769230769.23077</v>
+      </c>
+      <c r="E12" s="1">
+        <f>0.75*C12</f>
+        <v>36000000</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.17</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E13" s="1"/>
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3400000000</v>
+      </c>
+      <c r="C13" s="1">
+        <v>79000000</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>1240875912.4087591</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>59250000</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.37</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
@@ -721,6 +767,9 @@
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>